<commit_message>
Daily Activity scrum call done
</commit_message>
<xml_diff>
--- a/AgileWork/Daily_Activity.xlsx
+++ b/AgileWork/Daily_Activity.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sa356713/git/SOWER/AgileWork/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19320" windowHeight="6345" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
     <sheet name="Sep" sheetId="1" r:id="rId2"/>
     <sheet name="Tasks" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>Travel</t>
   </si>
@@ -227,13 +223,22 @@
   </si>
   <si>
     <t>Need to create StringGenerator, UniqueIdGenerator, NameGenerator, Address Generator , Double Generator, Primary key generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Done -- On Webservices, </t>
+  </si>
+  <si>
+    <t>Check Encryption on user front end</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,7 +335,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -365,7 +370,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -542,31 +547,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="3">
         <v>42984</v>
       </c>
@@ -580,7 +585,7 @@
         <v>42989</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -600,7 +605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -623,7 +628,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -643,7 +648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -663,7 +668,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -683,7 +688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="D7" t="s">
         <v>23</v>
       </c>
@@ -700,7 +705,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -717,7 +722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -740,21 +745,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4">
         <v>42983</v>
       </c>
@@ -766,7 +771,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0.39583333333333331</v>
       </c>
@@ -786,7 +791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>0.4375</v>
       </c>
@@ -797,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>0.54166666666666663</v>
       </c>
@@ -808,7 +813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>0.59027777777777779</v>
       </c>
@@ -828,7 +833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>0.125</v>
       </c>
@@ -839,7 +844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>0.16666666666666666</v>
       </c>
@@ -859,7 +864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>0.22222222222222221</v>
       </c>
@@ -889,25 +894,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="109.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="109.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -930,7 +935,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -945,7 +950,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -954,7 +959,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -963,7 +968,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -975,7 +980,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -987,7 +992,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1004,7 +1009,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1018,7 +1023,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1032,7 +1037,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1045,8 +1050,11 @@
       <c r="D10" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1058,7 +1066,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1073,7 +1081,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1081,7 +1089,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1089,7 +1097,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1097,42 +1105,48 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23">
         <v>22</v>
       </c>

</xml_diff>